<commit_message>
Update after review with EMUS team
Signed-off-by: Mike Thompson <mike@openhwgroup.org>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/SimulationVerificationPlan/base_instruction_set/CV32E40P_instruction_exceptions.xlsx
+++ b/verif/CV32E40P/SimulationVerificationPlan/base_instruction_set/CV32E40P_instruction_exceptions.xlsx
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="282">
   <si>
     <t xml:space="preserve">Requirement Location</t>
   </si>
@@ -680,6 +680,9 @@
 (partial coverage)</t>
   </si>
   <si>
+    <t xml:space="preserve">DavidMcD has script that he can use to cover all illegal instructions.   (Requires use of EM custom exception handler.)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISA
 Chapter 2.2 &amp; 2.5</t>
   </si>
@@ -739,6 +742,9 @@
     <t xml:space="preserve">general_exception_test</t>
   </si>
   <si>
+    <t xml:space="preserve">Covered in em test</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISA
 Chapter 2.6</t>
   </si>
@@ -758,7 +764,7 @@
     <t xml:space="preserve">Assertion Coverage</t>
   </si>
   <si>
-    <t xml:space="preserve">Coverage of misaligned load/store on memory interface</t>
+    <t xml:space="preserve">Not covered</t>
   </si>
   <si>
     <t xml:space="preserve">ISA
@@ -856,7 +862,8 @@
     <t xml:space="preserve">Demonstrate that all illegal CSR accesses generate an exception.</t>
   </si>
   <si>
-    <t xml:space="preserve">This is an overlap with the CSR DV plan.</t>
+    <t xml:space="preserve">Partial coverage
+Covered in CSR DV Plan </t>
   </si>
   <si>
     <t xml:space="preserve">CSR Fields NOT Implemented</t>
@@ -907,6 +914,9 @@
   </si>
   <si>
     <t xml:space="preserve">All exception jump to the base address of mtvec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial coverage</t>
   </si>
   <si>
     <t xml:space="preserve">ISA-P
@@ -981,7 +991,11 @@
     <t xml:space="preserve">Counters function as expected and give the EXACT count expected.</t>
   </si>
   <si>
-    <t xml:space="preserve">ISS does not model alll counters</t>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISS does not model all counters
+Covered in Performance Counter tests</t>
   </si>
   <si>
     <t xml:space="preserve">ISA-P
@@ -1038,6 +1052,9 @@
     <t xml:space="preserve">When interrupt or exception occurs, mepc is loaded with proper pc value to return to</t>
   </si>
   <si>
+    <t xml:space="preserve">Success-case (partial) coverage</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISA-P
 Chapter 3.1.16</t>
   </si>
@@ -1054,7 +1071,7 @@
     <t xml:space="preserve">The expected cause value is found in the mcause register when exceptions happen.</t>
   </si>
   <si>
-    <t xml:space="preserve">Constrained-Random</t>
+    <t xml:space="preserve">All mcause exception codes are tested for.  Do not test for mcause codes under interrupt conditions</t>
   </si>
   <si>
     <t xml:space="preserve">ISA-P
@@ -1151,6 +1168,9 @@
     <t xml:space="preserve">Ecall, ebreak, and c.ebreak all generate the appropriate exceptions</t>
   </si>
   <si>
+    <t xml:space="preserve">Covered</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISA-DEBUG Chapter 4.8.1</t>
   </si>
   <si>
@@ -1164,6 +1184,9 @@
   </si>
   <si>
     <t xml:space="preserve">Internal signal riscv_core/debug_mode=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered in Debug DV Plan</t>
   </si>
   <si>
     <t xml:space="preserve">ISA-P Chapter 3.3</t>
@@ -1413,7 +1436,7 @@
     <t xml:space="preserve">Assertion Check</t>
   </si>
   <si>
-    <t xml:space="preserve">N/A</t>
+    <t xml:space="preserve">Constrained-Random</t>
   </si>
   <si>
     <t xml:space="preserve">Any/All</t>
@@ -1611,7 +1634,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1686,6 +1709,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1805,28 +1832,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:AMJ127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="17.01953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="33.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="10" style="1" width="17"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1854,8 +1881,9 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1878,7 +1906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -1903,22 +1931,25 @@
       <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="180" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>14</v>
@@ -1927,287 +1958,293 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="57.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="120" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="105" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="I14" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="I15" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="46.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>22</v>
@@ -2215,165 +2252,173 @@
       <c r="H16" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="7"/>
       <c r="I17" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="I19" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="46.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="I20" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="I21" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="57.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G22" s="7"/>
       <c r="I22" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>22</v>
@@ -2381,314 +2426,335 @@
       <c r="H23" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I23" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>140</v>
+        <v>14</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I24" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="7"/>
       <c r="G25" s="2"/>
       <c r="I25" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="I26" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="I28" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="I29" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>22</v>
       </c>
       <c r="H31" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I31" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>22</v>
       </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="57.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G34" s="15" t="s">
         <v>22</v>
       </c>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>22</v>
       </c>
       <c r="H35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>22</v>
       </c>
       <c r="H36" s="2"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" s="18" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="17" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -2698,546 +2764,547 @@
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
-    </row>
-    <row r="39" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G40" s="15" t="s">
         <v>22</v>
       </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F113" s="7"/>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F114" s="7"/>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F115" s="7"/>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F116" s="7"/>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F117" s="7"/>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F118" s="7"/>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F119" s="7"/>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F120" s="7"/>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F121" s="7"/>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F122" s="7"/>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F123" s="7"/>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F124" s="7"/>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F125" s="7"/>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F126" s="7"/>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F127" s="7"/>
     </row>
   </sheetData>
@@ -3276,31 +3343,31 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>241</v>
+      <c r="B2" s="19" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="0" t="s">
-        <v>242</v>
+      <c r="C3" s="19" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
-        <v>243</v>
+      <c r="C4" s="19" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>244</v>
+      <c r="B6" s="19" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>245</v>
+      <c r="B8" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3325,103 +3392,103 @@
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="19.3"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="19" t="s">
+      <c r="A2" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="A3" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>251</v>
+      <c r="A4" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="A5" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>47</v>
+      <c r="E5" s="19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>254</v>
+      <c r="A6" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>256</v>
+      <c r="A7" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>129</v>
+      <c r="A8" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>258</v>
+      <c r="A9" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>256</v>
+      <c r="A10" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3446,325 +3513,325 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="14.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>259</v>
+      <c r="A1" s="19" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>260</v>
+      <c r="A2" s="19" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>261</v>
+      <c r="A3" s="19" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22" t="s">
+      <c r="A5" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>265</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>266</v>
-      </c>
-      <c r="E6" s="22"/>
+      <c r="A6" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="n">
+      <c r="A7" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="B7" s="24" t="n">
+      <c r="B7" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="24" t="n">
+      <c r="C7" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="24" t="n">
+      <c r="D7" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>267</v>
+      <c r="E7" s="26" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="n">
+      <c r="A8" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="B8" s="26" t="n">
+      <c r="B8" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="26" t="n">
+      <c r="C8" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="26" t="n">
+      <c r="D8" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>268</v>
+      <c r="E8" s="26" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="n">
+      <c r="A9" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="B9" s="26" t="n">
+      <c r="B9" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="26" t="n">
+      <c r="C9" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="26" t="n">
+      <c r="D9" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>268</v>
+      <c r="E9" s="26" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="n">
+      <c r="A10" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="B10" s="27" t="n">
+      <c r="B10" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="27" t="n">
+      <c r="C10" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="27" t="n">
+      <c r="D10" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>269</v>
+      <c r="E10" s="26" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26" t="n">
+      <c r="A11" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="B11" s="26" t="n">
+      <c r="B11" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="26" t="n">
+      <c r="C11" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="D11" s="26" t="n">
+      <c r="D11" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>268</v>
+      <c r="E11" s="26" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="n">
+      <c r="A12" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="B12" s="24" t="n">
+      <c r="B12" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="24" t="n">
+      <c r="C12" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="24" t="n">
+      <c r="D12" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>270</v>
+      <c r="E12" s="26" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28" t="n">
+      <c r="A13" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="B13" s="28" t="n">
+      <c r="B13" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="28" t="n">
+      <c r="C13" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="28" t="n">
+      <c r="D13" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>271</v>
+      <c r="E13" s="26" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="n">
+      <c r="A14" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="B14" s="24" t="n">
+      <c r="B14" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="24" t="n">
+      <c r="C14" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="24" t="n">
+      <c r="D14" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>270</v>
+      <c r="E14" s="26" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26" t="n">
+      <c r="A15" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="B15" s="26" t="n">
+      <c r="B15" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="C15" s="26" t="n">
+      <c r="C15" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="26" t="n">
+      <c r="D15" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="25" t="s">
-        <v>268</v>
+      <c r="E15" s="26" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="n">
+      <c r="A16" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="24" t="n">
+      <c r="B16" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="C16" s="24" t="n">
+      <c r="C16" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="24" t="n">
+      <c r="D16" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="25" t="s">
-        <v>272</v>
+      <c r="E16" s="26" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="n">
+      <c r="A17" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="27" t="n">
+      <c r="B17" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="C17" s="27" t="n">
+      <c r="C17" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="27" t="n">
+      <c r="D17" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="E17" s="25" t="s">
-        <v>273</v>
+      <c r="E17" s="26" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="n">
+      <c r="A18" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="24" t="n">
+      <c r="B18" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="24" t="n">
+      <c r="C18" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="24" t="n">
+      <c r="D18" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="25" t="s">
-        <v>272</v>
+      <c r="E18" s="26" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="n">
+      <c r="A19" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="24" t="n">
+      <c r="B19" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="C19" s="24" t="n">
+      <c r="C19" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="D19" s="24" t="n">
+      <c r="D19" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="25" t="s">
-        <v>274</v>
+      <c r="E19" s="26" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="n">
+      <c r="A20" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="B20" s="24" t="n">
+      <c r="B20" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="24" t="n">
+      <c r="C20" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="24" t="n">
+      <c r="D20" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="25" t="s">
-        <v>274</v>
+      <c r="E20" s="26" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="n">
+      <c r="A21" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="B21" s="24" t="n">
+      <c r="B21" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="C21" s="24" t="n">
+      <c r="C21" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="24" t="n">
+      <c r="D21" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="25" t="s">
-        <v>274</v>
+      <c r="E21" s="26" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="n">
+      <c r="A22" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="B22" s="24" t="n">
+      <c r="B22" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="C22" s="24" t="n">
+      <c r="C22" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="24" t="n">
+      <c r="D22" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="25" t="s">
-        <v>274</v>
+      <c r="E22" s="26" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>